<commit_message>
Commit: Merging levels V2
</commit_message>
<xml_diff>
--- a/DERIVED/combineLevels_train_processed.xlsx
+++ b/DERIVED/combineLevels_train_processed.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\system5\Documents\StudyWork\Kaggle\House_Pricing\DERIVED\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20500" windowHeight="7760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20505" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="summary_train_processed" sheetId="1" r:id="rId1"/>
@@ -2247,7 +2252,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2257,27 +2262,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="58" max="59" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" s="2" customFormat="1">
+    <row r="1" spans="1:79" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2510,7 +2518,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:79">
+    <row r="2" spans="1:79" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>134</v>
       </c>
@@ -2743,7 +2751,7 @@
         <v>0.34236111111111112</v>
       </c>
     </row>
-    <row r="3" spans="1:79">
+    <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>197</v>
       </c>
@@ -2976,7 +2984,7 @@
         <v>0.25347222222222221</v>
       </c>
     </row>
-    <row r="4" spans="1:79">
+    <row r="4" spans="1:79" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>262</v>
       </c>
@@ -3209,7 +3217,7 @@
         <v>0.66805555555555551</v>
       </c>
     </row>
-    <row r="5" spans="1:79">
+    <row r="5" spans="1:79" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>331</v>
       </c>
@@ -3442,7 +3450,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:79">
+    <row r="6" spans="1:79" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>386</v>
       </c>
@@ -3675,7 +3683,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:79">
+    <row r="7" spans="1:79" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>437</v>
       </c>
@@ -3908,7 +3916,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="8" spans="1:79">
+    <row r="8" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>232</v>
       </c>
@@ -4138,7 +4146,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="9" spans="1:79">
+    <row r="9" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>456</v>
       </c>
@@ -4174,7 +4182,7 @@
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
     </row>
-    <row r="10" spans="1:79">
+    <row r="10" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>457</v>
       </c>
@@ -4208,7 +4216,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="13" spans="1:79">
+    <row r="13" spans="1:79" x14ac:dyDescent="0.25">
       <c r="V13" s="4"/>
       <c r="W13" s="4"/>
       <c r="X13" s="4"/>
@@ -4268,7 +4276,7 @@
       <c r="BZ13" s="4"/>
       <c r="CA13" s="4"/>
     </row>
-    <row r="14" spans="1:79">
+    <row r="14" spans="1:79" x14ac:dyDescent="0.25">
       <c r="V14" s="4"/>
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>

</xml_diff>

<commit_message>
Commit: Grid search xgb and rf
</commit_message>
<xml_diff>
--- a/DERIVED/combineLevels_train_processed.xlsx
+++ b/DERIVED/combineLevels_train_processed.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="summary_train_processed" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2262,8 +2262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="BI1" workbookViewId="0">
+      <selection activeCell="AJ10" sqref="AJ10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2279,10 +2279,15 @@
     <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11" bestFit="1" customWidth="1"/>
     <col min="58" max="59" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:79" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4214,6 +4219,16 @@
       </c>
       <c r="T10" s="4" t="s">
         <v>452</v>
+      </c>
+      <c r="AI10" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="AJ10" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="AK10" s="4"/>
+      <c r="AL10" s="4" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="13" spans="1:79" x14ac:dyDescent="0.25">
@@ -4291,16 +4306,6 @@
       <c r="AG14" s="4"/>
       <c r="AH14" s="4"/>
       <c r="AI14" s="4"/>
-      <c r="AJ14" s="4" t="s">
-        <v>461</v>
-      </c>
-      <c r="AK14" s="4" t="s">
-        <v>462</v>
-      </c>
-      <c r="AL14" s="4"/>
-      <c r="AM14" s="4" t="s">
-        <v>463</v>
-      </c>
       <c r="AN14" s="4"/>
       <c r="AO14" s="4"/>
       <c r="AP14" s="4"/>
@@ -4344,7 +4349,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>